<commit_message>
se agregaron los cambios finales
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -37,19 +37,19 @@
     <t>Participante</t>
   </si>
   <si>
-    <t>Cree el nuevo repositorio</t>
-  </si>
-  <si>
-    <t>Cree el proyecto y la aplicación</t>
-  </si>
-  <si>
-    <t>Cree la carpeta static y agrega las imágenes, css, js</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comencé a adaptar el proyecto a Django </t>
-  </si>
-  <si>
-    <t>comence a programar las nuevas paginas de carrito y comprar</t>
+    <t>Se creo el nuevo repositorio</t>
+  </si>
+  <si>
+    <t>Se creo el proyecto y la aplicación</t>
+  </si>
+  <si>
+    <t>se creo la carpeta static y agrega las imágenes, css, js</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se comenzo a adaptar el proyecto a Django </t>
+  </si>
+  <si>
+    <t>Se comenzó a programar las nuevas paginas de carrito y comprar</t>
   </si>
   <si>
     <t>Se comenzó a programar el CRUD</t>
@@ -61,16 +61,16 @@
     <t>Se programo la opción de Delete del CRUD</t>
   </si>
   <si>
-    <t>Se programo la opción de Créate del CRUD en el formulario para agregar productos</t>
-  </si>
-  <si>
-    <t>Se programo la opcion de Update del CRUD en el formulario para modificar productos</t>
-  </si>
-  <si>
-    <t>Se arreglaron detalles del proyecto</t>
-  </si>
-  <si>
-    <t>Se realizo el commit final</t>
+    <t>Se programo la opción de Créate del CRUD en el formulario para agregar un producto</t>
+  </si>
+  <si>
+    <t>Se programo la opcion de Update del CRUD en el formulario para modificar un producto</t>
+  </si>
+  <si>
+    <t>Se arreglaron algunos detalles del proyecto</t>
+  </si>
+  <si>
+    <t>Se realizo el ultimo commit</t>
   </si>
 </sst>
 </file>
@@ -1256,7 +1256,7 @@
   <cols>
     <col min="1" max="1" width="10.8516" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.6719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="65.1719" style="1" customWidth="1"/>
+    <col min="3" max="3" width="66.6719" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.8516" style="1" customWidth="1"/>
     <col min="6" max="16384" width="10.8516" style="1" customWidth="1"/>

</xml_diff>